<commit_message>
new framework structure changes
</commit_message>
<xml_diff>
--- a/testData/EvaticTestData.xlsx
+++ b/testData/EvaticTestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evatic365-my.sharepoint.com/personal/rajan_jeyaraj_asolvi_com/Documents/Rajan/Rajan/Projects/EvaticAutomation/testData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://evatic365-my.sharepoint.com/personal/rajan_jeyaraj_asolvi_com/Documents/Rajan/Rajan/Projects/04.EvaticAutomation-Collide/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="434" documentId="11_F25DC773A252ABDACC1048E0711B65C25ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FB79E71-D151-46F1-9F1E-F8AE9014800A}"/>
+  <xr:revisionPtr revIDLastSave="735" documentId="11_F25DC773A252ABDACC1048E0711B65C25ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9699516-5957-4040-826D-F7E83DBA7DF0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,9 @@
     <sheet name="Project" sheetId="4" r:id="rId4"/>
     <sheet name="Order" sheetId="5" r:id="rId5"/>
     <sheet name="SalesProject" sheetId="6" r:id="rId6"/>
+    <sheet name="Contract" sheetId="9" r:id="rId7"/>
+    <sheet name="CustWeb" sheetId="7" r:id="rId8"/>
+    <sheet name="AdminWeb" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="152">
   <si>
     <t>TestCaseId</t>
   </si>
@@ -170,9 +173,6 @@
     <t>TC_001_Evatic_Regression_ProjectModule</t>
   </si>
   <si>
-    <t>100001</t>
-  </si>
-  <si>
     <t>PackingSlipNo</t>
   </si>
   <si>
@@ -185,9 +185,6 @@
     <t>TC_001_Evatic_Regression_OrderModule</t>
   </si>
   <si>
-    <t>BT001</t>
-  </si>
-  <si>
     <t>ELH2701E</t>
   </si>
   <si>
@@ -218,9 +215,6 @@
     <t>QuanToMve</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>TC_001_Evatic_Regression_SalesProjectModule</t>
   </si>
   <si>
@@ -239,10 +233,262 @@
     <t>RajanCust001</t>
   </si>
   <si>
-    <t>09/12/2023</t>
-  </si>
-  <si>
-    <t>150</t>
+    <t>VisitName</t>
+  </si>
+  <si>
+    <t>Address1</t>
+  </si>
+  <si>
+    <t>Breidablikkveien 6</t>
+  </si>
+  <si>
+    <t>52345345</t>
+  </si>
+  <si>
+    <t>1167 Oslo</t>
+  </si>
+  <si>
+    <t>RajanCustomer</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>TestFirstName TestLastName</t>
+  </si>
+  <si>
+    <t>TestFirstName</t>
+  </si>
+  <si>
+    <t>TestLastName</t>
+  </si>
+  <si>
+    <t>99999999</t>
+  </si>
+  <si>
+    <t>SymCode</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>RefNo</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>TestTitle1</t>
+  </si>
+  <si>
+    <t>TestRef1</t>
+  </si>
+  <si>
+    <t>TestDesc1</t>
+  </si>
+  <si>
+    <t>TC_007_Evatic_Regression_CustWebModule_001</t>
+  </si>
+  <si>
+    <t>TC_007_Evatic_Regression_CustOrderModule_002</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>InvoiceAddress</t>
+  </si>
+  <si>
+    <t>karsvesvingen 5</t>
+  </si>
+  <si>
+    <t>SerSymCode</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Mach</t>
+  </si>
+  <si>
+    <t>Dept</t>
+  </si>
+  <si>
+    <t>RJMach</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>CP3000</t>
+  </si>
+  <si>
+    <t>MacAddress</t>
+  </si>
+  <si>
+    <t>MacBrand</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>TC_007_Evatic_Regression_CustMachineModule_003</t>
+  </si>
+  <si>
+    <t>TC_007_Evatic_Regression_CustContactsModule_004</t>
+  </si>
+  <si>
+    <t>ConJobTitle</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>ConTitle</t>
+  </si>
+  <si>
+    <t>test1.test1@asolvi.com</t>
+  </si>
+  <si>
+    <t>ConFaxNum</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>TC_008_Evatic_Regression_AdminWebModule_001</t>
+  </si>
+  <si>
+    <t>TC_008_Evatic_Regression_AdminWebNewRoles_002</t>
+  </si>
+  <si>
+    <t>RoleDesc</t>
+  </si>
+  <si>
+    <t>RoleName</t>
+  </si>
+  <si>
+    <t>TestRole</t>
+  </si>
+  <si>
+    <t>TestRoleDesc</t>
+  </si>
+  <si>
+    <t>TC_001_Evatic_Regression_ContractModule</t>
+  </si>
+  <si>
+    <t>CustNo</t>
+  </si>
+  <si>
+    <t>Technician</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>RJMachine001</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>02/27/2024</t>
+  </si>
+  <si>
+    <t>RJBeast01</t>
+  </si>
+  <si>
+    <t>TC_002_Evatic_Regression_OrderModule</t>
+  </si>
+  <si>
+    <t>TC_003_Evatic_Regression_OrderModule</t>
+  </si>
+  <si>
+    <t>SerialNo</t>
+  </si>
+  <si>
+    <t>MAGTONER</t>
+  </si>
+  <si>
+    <t>CalculationType1</t>
+  </si>
+  <si>
+    <t>CalculationType2</t>
+  </si>
+  <si>
+    <t>ContractTemplate</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>Factor</t>
+  </si>
+  <si>
+    <t>0.01</t>
+  </si>
+  <si>
+    <t>002 - Leasing</t>
+  </si>
+  <si>
+    <t>AllinVol</t>
+  </si>
+  <si>
+    <t>0.02</t>
+  </si>
+  <si>
+    <t>0.04</t>
+  </si>
+  <si>
+    <t>PpeuBlack</t>
+  </si>
+  <si>
+    <t>PpeuColor</t>
+  </si>
+  <si>
+    <t>qa.qa</t>
+  </si>
+  <si>
+    <t>qa</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>10000</t>
+  </si>
+  <si>
+    <t>TC_002_Evatic_Regression_ProjectModule</t>
+  </si>
+  <si>
+    <t>SB</t>
+  </si>
+  <si>
+    <t>RJ004</t>
   </si>
 </sst>
 </file>
@@ -274,7 +520,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -297,17 +543,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,8 +864,8 @@
     <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -646,28 +906,28 @@
         <v>44</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="N1" s="4" t="s">
-        <v>55</v>
-      </c>
       <c r="O1" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -705,7 +965,7 @@
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -717,34 +977,34 @@
         <v>40</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>43</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>70</v>
+        <v>124</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="Q3" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="R3" s="2" t="s">
-        <v>62</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -764,7 +1024,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
@@ -850,8 +1110,381 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8383C2-B57C-4433-B9BA-AFE6447C28E6}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54A3F9B-6305-46ED-9A3D-F6A6ECA5D32B}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9380B9E-7837-415A-AB0A-EEA772172D92}">
+  <dimension ref="A1:L2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FD86EC6-AF8B-44DD-8BE8-BD15102E0BD3}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -861,67 +1494,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D1" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA8383C2-B57C-4433-B9BA-AFE6447C28E6}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>31</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -934,10 +1507,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>120</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
@@ -953,49 +1526,477 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F54A3F9B-6305-46ED-9A3D-F6A6ECA5D32B}">
-  <dimension ref="A1:J2"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E93358E-D7CF-4402-A03A-49DD60879E16}">
+  <dimension ref="A1:AT5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="R1" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="5"/>
+      <c r="AM3" s="5"/>
+      <c r="AN3" s="5"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="5"/>
+      <c r="AQ3" s="5"/>
+      <c r="AR3" s="5"/>
+      <c r="AS3" s="5"/>
+      <c r="AT3" s="5"/>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5"/>
+      <c r="AN4" s="5"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="5"/>
+      <c r="AQ4" s="5"/>
+      <c r="AR4" s="5"/>
+      <c r="AS4" s="5"/>
+      <c r="AT4" s="5"/>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y5" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z5" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CAE6800-4908-49CC-86E1-650F22DD3417}">
+  <dimension ref="A1:AT5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="12.85546875" customWidth="1"/>
+    <col min="18" max="18" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4"/>
       <c r="C1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="4"/>
+        <v>117</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
+      <c r="Y1" s="4"/>
+      <c r="Z1" s="4"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AD1" s="5"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5"/>
+      <c r="AK1" s="5"/>
+      <c r="AL1" s="5"/>
+      <c r="AM1" s="5"/>
+      <c r="AN1" s="5"/>
+      <c r="AO1" s="5"/>
+      <c r="AP1" s="5"/>
+      <c r="AQ1" s="5"/>
+      <c r="AR1" s="5"/>
+      <c r="AS1" s="5"/>
+      <c r="AT1" s="5"/>
+    </row>
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>52</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -1003,66 +2004,192 @@
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9380B9E-7837-415A-AB0A-EEA772172D92}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+    </row>
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+      <c r="W3" s="5"/>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5"/>
+      <c r="Z3" s="5"/>
+      <c r="AA3" s="5"/>
+      <c r="AB3" s="5"/>
+      <c r="AC3" s="5"/>
+      <c r="AD3" s="5"/>
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="5"/>
+      <c r="AH3" s="5"/>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5"/>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="5"/>
+      <c r="AM3" s="5"/>
+      <c r="AN3" s="5"/>
+      <c r="AO3" s="5"/>
+      <c r="AP3" s="5"/>
+      <c r="AQ3" s="5"/>
+      <c r="AR3" s="5"/>
+      <c r="AS3" s="5"/>
+      <c r="AT3" s="5"/>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5"/>
+      <c r="Z4" s="5"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="5"/>
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5"/>
+      <c r="AL4" s="5"/>
+      <c r="AM4" s="5"/>
+      <c r="AN4" s="5"/>
+      <c r="AO4" s="5"/>
+      <c r="AP4" s="5"/>
+      <c r="AQ4" s="5"/>
+      <c r="AR4" s="5"/>
+      <c r="AS4" s="5"/>
+      <c r="AT4" s="5"/>
+    </row>
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="5"/>
+      <c r="X5" s="2"/>
+      <c r="Y5" s="2"/>
+      <c r="Z5" s="2"/>
+      <c r="AA5" s="5"/>
+      <c r="AB5" s="5"/>
+      <c r="AC5" s="5"/>
+      <c r="AD5" s="5"/>
+      <c r="AE5" s="5"/>
+      <c r="AF5" s="5"/>
+      <c r="AG5" s="5"/>
+      <c r="AH5" s="5"/>
+      <c r="AI5" s="5"/>
+      <c r="AJ5" s="5"/>
+      <c r="AK5" s="5"/>
+      <c r="AL5" s="5"/>
+      <c r="AM5" s="5"/>
+      <c r="AN5" s="5"/>
+      <c r="AO5" s="5"/>
+      <c r="AP5" s="5"/>
+      <c r="AQ5" s="5"/>
+      <c r="AR5" s="5"/>
+      <c r="AS5" s="5"/>
+      <c r="AT5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>